<commit_message>
fix error on saving to existing xlsx and add future tests
</commit_message>
<xml_diff>
--- a/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
+++ b/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_01" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_02" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,10 +475,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>5.78</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="3">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>2.66</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="4">
@@ -517,10 +517,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="5">
@@ -538,10 +538,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="6">
@@ -559,10 +559,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>11.73</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="7">
@@ -580,10 +580,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>7.67</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>5.49</v>
       </c>
     </row>
     <row r="8">
@@ -601,10 +601,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>4.7</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="9">
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>15.48</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="10">
@@ -643,10 +643,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>14.32</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="11">
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3.38</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -685,10 +685,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>10.95</v>
       </c>
     </row>
     <row r="13">
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="14">
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>11.52</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>6.49</v>
       </c>
     </row>
     <row r="15">
@@ -748,10 +748,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>5.57</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="16">
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>20.33</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="18">
@@ -811,10 +811,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="19">
@@ -832,10 +832,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="20">
@@ -868,7 +868,6 @@
           <t>BONITO CONSERVA</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>0</v>
       </c>
@@ -891,10 +890,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>5.78</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>4.39</v>
       </c>
     </row>
     <row r="23">
@@ -912,10 +911,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2.84</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="24">
@@ -933,10 +932,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="25">
@@ -954,10 +953,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>1.72</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="26">
@@ -975,10 +974,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>3.12</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="27">
@@ -996,7 +995,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1.91</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -1017,10 +1016,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>10.73</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="29">
@@ -1038,10 +1037,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1.49</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="30">
@@ -1059,10 +1058,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>1.24</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="31">
@@ -1074,7 +1073,6 @@
           <t>CEREZAS</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
         <v>0</v>
       </c>
@@ -1097,10 +1095,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="33">
@@ -1118,10 +1116,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>2.12</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="34">
@@ -1139,10 +1137,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>6.11</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="35">
@@ -1160,10 +1158,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>4.42</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="36">
@@ -1175,7 +1173,6 @@
           <t xml:space="preserve">CIRUELAS </t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
         <v>0</v>
       </c>
@@ -1198,10 +1195,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>1.91</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1.09</v>
       </c>
     </row>
     <row r="38">
@@ -1219,10 +1216,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>2.73</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="39">
@@ -1234,7 +1231,6 @@
           <t>CORVINA FRESCA ENTERA</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
         <v>0</v>
       </c>
@@ -1257,10 +1253,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1.99</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="41">
@@ -1278,10 +1274,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>3.72</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="42">
@@ -1299,10 +1295,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="43">
@@ -1320,10 +1316,10 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>5.39</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>14.95</v>
       </c>
     </row>
     <row r="44">
@@ -1341,10 +1337,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>26.45</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="45">
@@ -1362,10 +1358,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>2.96</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="46">
@@ -1383,10 +1379,10 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>23.92</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="47">
@@ -1398,7 +1394,6 @@
           <t>ESPINACAS</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
         <v>0</v>
       </c>
@@ -1421,10 +1416,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>2.53</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="49">
@@ -1463,10 +1458,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>3.48</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="51">
@@ -1478,7 +1473,6 @@
           <t xml:space="preserve">GEL BAÑO </t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
         <v>0</v>
       </c>
@@ -1501,10 +1495,10 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>11.08</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="53">
@@ -1522,10 +1516,10 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>7.14</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="54">
@@ -1543,10 +1537,10 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>23.79</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="55">
@@ -1564,10 +1558,10 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>14.96</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="56">
@@ -1585,10 +1579,10 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="57">
@@ -1606,10 +1600,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="58">
@@ -1627,10 +1621,10 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>4.43</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>3.45</v>
       </c>
     </row>
     <row r="59">
@@ -1648,10 +1642,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="60">
@@ -1669,7 +1663,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>2.98</v>
       </c>
       <c r="E60" t="n">
         <v>0</v>
@@ -1690,10 +1684,10 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>10.95</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="62">
@@ -1711,10 +1705,10 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>3.98</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="63">
@@ -1732,10 +1726,10 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>5.7</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="64">
@@ -1753,10 +1747,10 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>4.42</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="65">
@@ -1774,10 +1768,10 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>14.56</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>13.99</v>
       </c>
     </row>
     <row r="66">
@@ -1795,10 +1789,10 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>14.56</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="67">
@@ -1816,10 +1810,10 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>4.54</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="68">
@@ -1837,10 +1831,10 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="69">
@@ -1858,10 +1852,10 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="70">
@@ -1879,7 +1873,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>1.24</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -1900,10 +1894,10 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>1.15</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="72">
@@ -1921,10 +1915,10 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>3.36</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>3.46</v>
       </c>
     </row>
     <row r="73">
@@ -1966,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="75">
@@ -1984,10 +1978,10 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>3.07</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="76">
@@ -1999,7 +1993,6 @@
           <t xml:space="preserve">LIMPIADOR VITROCERAMICA </t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
         <v>0</v>
       </c>
@@ -2022,10 +2015,10 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>5.32</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="78">
@@ -2043,10 +2036,10 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>14.99</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>16.95</v>
       </c>
     </row>
     <row r="79">
@@ -2064,10 +2057,10 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>2.96</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="80">
@@ -2106,10 +2099,10 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>14.2</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>3.39</v>
       </c>
     </row>
     <row r="82">
@@ -2127,10 +2120,10 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>2.2</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="83">
@@ -2148,10 +2141,10 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>1.82</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="84">
@@ -2169,10 +2162,10 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>5.23</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="85">
@@ -2190,10 +2183,10 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="86">
@@ -2205,7 +2198,6 @@
           <t>MEJILLON FRESCO</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
       <c r="D86" t="n">
         <v>0</v>
       </c>
@@ -2249,7 +2241,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>1.82</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -2270,7 +2262,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>10.24</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -2291,7 +2283,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>11.75</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -2312,7 +2304,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
@@ -2354,7 +2346,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -2375,7 +2367,7 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>20.91</v>
       </c>
       <c r="E94" t="n">
         <v>0</v>
@@ -2396,7 +2388,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>16.33</v>
       </c>
       <c r="E95" t="n">
         <v>0</v>
@@ -2417,7 +2409,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -2438,7 +2430,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -2459,7 +2451,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -2480,7 +2472,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>0.37</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
@@ -2501,7 +2493,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>4.38</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -2522,7 +2514,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>1.92</v>
       </c>
       <c r="E101" t="n">
         <v>0</v>
@@ -2543,7 +2535,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>18.17</v>
       </c>
       <c r="E102" t="n">
         <v>0</v>
@@ -2564,7 +2556,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>14.95</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
@@ -2585,7 +2577,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0</v>
+        <v>14.54</v>
       </c>
       <c r="E104" t="n">
         <v>0</v>
@@ -2606,7 +2598,7 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>0</v>
+        <v>4.18</v>
       </c>
       <c r="E105" t="n">
         <v>0</v>
@@ -2648,7 +2640,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>4.96</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -2669,7 +2661,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>3.62</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -2690,7 +2682,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>1.49</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -2711,7 +2703,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>15.64</v>
       </c>
       <c r="E110" t="n">
         <v>0</v>
@@ -2732,7 +2724,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>2.88</v>
       </c>
       <c r="E111" t="n">
         <v>0</v>
@@ -2753,7 +2745,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>7.78</v>
       </c>
       <c r="E112" t="n">
         <v>0</v>
@@ -2774,7 +2766,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="E113" t="n">
         <v>0</v>
@@ -2795,7 +2787,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>0</v>
+        <v>12.34</v>
       </c>
       <c r="E114" t="n">
         <v>0</v>
@@ -2816,7 +2808,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>0</v>
+        <v>4.9</v>
       </c>
       <c r="E115" t="n">
         <v>0</v>
@@ -2831,7 +2823,6 @@
           <t xml:space="preserve">QUESO EMMENTAL </t>
         </is>
       </c>
-      <c r="C116" t="inlineStr"/>
       <c r="D116" t="n">
         <v>0</v>
       </c>
@@ -2854,7 +2845,7 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>0</v>
+        <v>13.03</v>
       </c>
       <c r="E117" t="n">
         <v>0</v>
@@ -2869,7 +2860,6 @@
           <t>QUESO GOUDA TIERNO,</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr"/>
       <c r="D118" t="n">
         <v>0</v>
       </c>
@@ -2913,7 +2903,7 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0</v>
+        <v>32.25</v>
       </c>
       <c r="E120" t="n">
         <v>0</v>
@@ -2928,7 +2918,6 @@
           <t xml:space="preserve">SALMON FRESCO </t>
         </is>
       </c>
-      <c r="C121" t="inlineStr"/>
       <c r="D121" t="n">
         <v>0</v>
       </c>
@@ -2951,7 +2940,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="E122" t="n">
         <v>0</v>
@@ -2972,7 +2961,7 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>0</v>
+        <v>13.83</v>
       </c>
       <c r="E123" t="n">
         <v>0</v>
@@ -2993,7 +2982,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E124" t="n">
         <v>0</v>
@@ -3014,7 +3003,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>2.96</v>
       </c>
       <c r="E125" t="n">
         <v>0</v>
@@ -3056,7 +3045,7 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>2.88</v>
       </c>
       <c r="E127" t="n">
         <v>0</v>
@@ -3077,7 +3066,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>4.86</v>
       </c>
       <c r="E128" t="n">
         <v>0</v>
@@ -3098,7 +3087,7 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>3.94</v>
       </c>
       <c r="E129" t="n">
         <v>0</v>
@@ -3119,7 +3108,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>6.9</v>
       </c>
       <c r="E130" t="n">
         <v>0</v>
@@ -3140,7 +3129,7 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>7.96</v>
       </c>
       <c r="E131" t="n">
         <v>0</v>
@@ -3161,7 +3150,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>6.09</v>
       </c>
       <c r="E132" t="n">
         <v>0</v>
@@ -3182,7 +3171,7 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>1.32</v>
       </c>
       <c r="E133" t="n">
         <v>0</v>
@@ -3197,7 +3186,6 @@
           <t>ZUMO NARANJA</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr"/>
       <c r="D134" t="n">
         <v>0</v>
       </c>
@@ -3220,7 +3208,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E135" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
sending correct logs through email
</commit_message>
<xml_diff>
--- a/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
+++ b/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_02" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_03" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_10" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3669,7 +3670,6 @@
           <t>BONITO CONSERVA</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>0</v>
       </c>
@@ -3875,7 +3875,6 @@
           <t>CEREZAS</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
         <v>0</v>
       </c>
@@ -3976,7 +3975,6 @@
           <t xml:space="preserve">CIRUELAS </t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
         <v>0</v>
       </c>
@@ -4035,7 +4033,6 @@
           <t>CORVINA FRESCA ENTERA</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
         <v>0</v>
       </c>
@@ -4199,7 +4196,6 @@
           <t>ESPINACAS</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
         <v>0</v>
       </c>
@@ -4279,7 +4275,6 @@
           <t xml:space="preserve">GEL BAÑO </t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
         <v>0</v>
       </c>
@@ -4800,7 +4795,6 @@
           <t xml:space="preserve">LIMPIADOR VITROCERAMICA </t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
         <v>0</v>
       </c>
@@ -5006,7 +5000,6 @@
           <t>MEJILLON FRESCO</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
       <c r="D86" t="n">
         <v>0</v>
       </c>
@@ -5632,7 +5625,6 @@
           <t xml:space="preserve">QUESO EMMENTAL </t>
         </is>
       </c>
-      <c r="C116" t="inlineStr"/>
       <c r="D116" t="n">
         <v>0</v>
       </c>
@@ -5656,6 +5648,2815 @@
       </c>
       <c r="D117" t="n">
         <v>13.03</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>QUESO GOUDA TIERNO,</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO </t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>SALMON AHUMADO LONCHAS</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SALMON FRESCO </t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SALSA BECHAMEL </t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>SARDINA ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>13.83</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUAVIZANTE ROPA CONCENTRADO </t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>dosis</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>TALLARINES</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>TOMATE  CHERRY</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>TOMATE ENSALADA</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>TOMATE FRITO ACEITE OLIVA RECETA ARTESANA</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>TOMATE PERA</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>VINAGRE BALSAMICO MODENA</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>VINAGRE JEREZ</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>7.96</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>YOGUR GRIEGO NATURAL</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>ZANAHORIA</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>ZUMO NARANJA</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JABON MANOS LIQUIDO </t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E135"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PRODUCTOS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>UNIDADES</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Eroski</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ABRILLANTADOR LAVAVAJILLAS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ACEITE GIRASOL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ACEITUNA NEGRA SIN HUESO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>13</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.07</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ACEITUNA RELLENA ANCHOA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>11.73</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGUACATE </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7.67</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AJO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALCACHOFA CORAZONES GRANDES </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>15.48</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALMENDRA CRUDA </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>15.03</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ALUBIA COCIDA BLANCA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ANCHOA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>15.96</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12.95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ANCHOA FILETE ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ARANDANOS </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ARROZ BOMBA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ATUN CLARO EN ACEITE OLIVA </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AVELLANA TOSTADA PELADA SIN SA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>20.33</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.49</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AZUCAR BLANQUILLA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BOLSA BASURA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BONITO </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BONITO CONSERVA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BORRAJA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BROCOLI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CACAHUETE TOSTADO </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CALABACIN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CALABAZA</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CALABAZA CACAHUETE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CARNE PICADA VACUNO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>10.73</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CEBOLLA BLANCA</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CEBOLLETA </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>manojo</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CEREZAS</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CERVEZA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CERVEZA 0</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CHAMPIÑON ENTERO CONSERVA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>6.11</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CHAMPIÑONES</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CIRUELAS </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>COGOLLOS CORAZONES</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>COLIFROR</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CORVINA FRESCA ENTERA</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>DENTRIFICO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>DESENGRASANTE  KH-7</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>DETERGENTE LIQUIDO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>dosis</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>DORADA FRESCA ENTERA</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="E43" t="n">
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ENTRECOT</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>26.45</v>
+      </c>
+      <c r="E44" t="n">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ESPAGUETI PASTA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESPARRAGO BLANCO MUY GRUESO 6/12 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>23.92</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ESPINACAS</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ESPUMA AFEITAR</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>FAIRY</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>GARBANZO COCIDO</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GEL BAÑO </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>GUINDILLAS</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>11.08</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>GUISANTE CONSERVA</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GULAS </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>23.79</v>
+      </c>
+      <c r="E54" t="n">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HAMBURGUESA VACUNO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="E55" t="n">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>HAMBURGUESA VACUNO/CERDO</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>HARINA TRIGO</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HUEVOS CAMPEROS </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HUEVOS CODORNIZ</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HUEVOS XL</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>JAMON COCIDO EXTRA LONCHAS</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>10.95</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JUDIA VERDE PLANA </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>KETCHUP</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>KIWI VERDE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="E64" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LANGOSTINO </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="E65" t="n">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LANGOSTINO COCIDO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="E66" t="n">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LAVAVAJILLAS MAQUINA GEL </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="E67" t="n">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>LECHE DESNATADA</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>LECHE SEMIDESNATADA</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LECHUGA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LEGIA </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="E71" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>LENTEJA PARDINA</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="E72" t="n">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>LIMON</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LIMPIACRISTALES</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LIMPIADOR SUELO</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LIMPIADOR VITROCERAMICA </t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>LONGANIZA FRESCO</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>5.32</v>
+      </c>
+      <c r="E77" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LUBINA FRESCA ENTERA </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MACARRON PASTA DE TRIGO</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MANDARINA</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MANTEQUILLA </t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="E81" t="n">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MANZANA FUYI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>MANZANA GOLDEN</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>MAYONESA</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>5.23</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEJILLON ESCABECHE 8/12 PIEZAS EN ACEITE OLIVA </t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E85" t="n">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MEJILLON FRESCO</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MELOCOTON </t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MELON</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MENESTRA VERDURA CONSERVA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MERLUZA FRESCA ENTERA </t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>13.95</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MOSTAZA</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>NARANJA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NATA COCINA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NUEZ </t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>21.94</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>PANCETA LONCHAS</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>16.33</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PAÑUELOS PAPEL BOLSILLO</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PAPEL ALUMINIO </t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>metro</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>PAPEL COCINA BLANCO DOBLE</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>rollo</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>PAPEL HIGIENICO DOBLE ROLLO 2 CAPAS</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>rollo</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>8.99</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>PATATA ENTERA CONSERVA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>PATATA NUEVA</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PAVO </t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>19.13</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PECHUGA PAVO </t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>14.95</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>PEPINILLOS</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>14.54</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>PIMIENTO ASADO TIRAS</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PIMIENTO ITALIANO </t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>PIMIENTO PIQUILLO ASADO ENTERO</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>PIMIENTO ROJO</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>PIÑA</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>PIPAS GIRASOL GIGANTES TOSTADAS CON SAL</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>15.64</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>PLATANO CANARIO</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>POCHA  COCIDA</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>7.78</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>POLLO ENTERO LIMPIO FRESCO</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>POLLO PECHUGA FILETES FRESCO</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>12.34</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUERRO </t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QUESO EMMENTAL </t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QUESO FRESCO </t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>13.17</v>
       </c>
       <c r="E117" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Working SMTP script with multiple receivers, added configuration in TOML format
</commit_message>
<xml_diff>
--- a/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
+++ b/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_02" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_03" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_10" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_15" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -6470,7 +6471,6 @@
           <t>BONITO CONSERVA</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>0</v>
       </c>
@@ -6676,7 +6676,6 @@
           <t>CEREZAS</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
         <v>0</v>
       </c>
@@ -6777,7 +6776,6 @@
           <t xml:space="preserve">CIRUELAS </t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
         <v>0</v>
       </c>
@@ -6836,7 +6834,6 @@
           <t>CORVINA FRESCA ENTERA</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
         <v>0</v>
       </c>
@@ -7000,7 +6997,6 @@
           <t>ESPINACAS</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
         <v>0</v>
       </c>
@@ -7080,7 +7076,6 @@
           <t xml:space="preserve">GEL BAÑO </t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
         <v>0</v>
       </c>
@@ -7601,7 +7596,6 @@
           <t xml:space="preserve">LIMPIADOR VITROCERAMICA </t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
         <v>0</v>
       </c>
@@ -7807,7 +7801,6 @@
           <t>MEJILLON FRESCO</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
       <c r="D86" t="n">
         <v>0</v>
       </c>
@@ -8083,6 +8076,2814 @@
       </c>
       <c r="D99" t="n">
         <v>8.99</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>PATATA ENTERA CONSERVA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>PATATA NUEVA</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PAVO </t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>19.13</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PECHUGA PAVO </t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>14.95</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>PEPINILLOS</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>14.54</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>PIMIENTO ASADO TIRAS</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PIMIENTO ITALIANO </t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>PIMIENTO PIQUILLO ASADO ENTERO</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>PIMIENTO ROJO</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>PIÑA</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>PIPAS GIRASOL GIGANTES TOSTADAS CON SAL</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>15.64</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>PLATANO CANARIO</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>POCHA  COCIDA</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>7.78</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>POLLO ENTERO LIMPIO FRESCO</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>POLLO PECHUGA FILETES FRESCO</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>12.34</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUERRO </t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QUESO EMMENTAL </t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QUESO FRESCO </t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>QUESO GOUDA TIERNO,</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO </t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>SALMON AHUMADO LONCHAS</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SALMON FRESCO </t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SALSA BECHAMEL </t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>SARDINA ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>13.83</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUAVIZANTE ROPA CONCENTRADO </t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>dosis</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>TALLARINES</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>TOMATE  CHERRY</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>TOMATE ENSALADA</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>TOMATE FRITO ACEITE OLIVA RECETA ARTESANA</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>TOMATE PERA</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>VINAGRE BALSAMICO MODENA</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>VINAGRE JEREZ</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>7.96</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>YOGUR GRIEGO NATURAL</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>ZANAHORIA</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>ZUMO NARANJA</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JABON MANOS LIQUIDO </t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E135"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PRODUCTOS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>UNIDADES</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Eroski</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ABRILLANTADOR LAVAVAJILLAS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ACEITE GIRASOL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ACEITUNA NEGRA SIN HUESO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>13</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.07</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ACEITUNA RELLENA ANCHOA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>11.73</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGUACATE </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7.67</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AJO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALCACHOFA CORAZONES GRANDES </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>15.48</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALMENDRA CRUDA </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>15.03</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ALUBIA COCIDA BLANCA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ANCHOA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ANCHOA FILETE ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ARANDANOS </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ARROZ BOMBA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ATUN CLARO EN ACEITE OLIVA </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AVELLANA TOSTADA PELADA SIN SA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>20.33</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.49</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AZUCAR BLANQUILLA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BOLSA BASURA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BONITO </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>22.95</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BONITO CONSERVA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BORRAJA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BROCOLI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CACAHUETE TOSTADO </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CALABACIN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CALABAZA</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.07</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CALABAZA CACAHUETE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CARNE PICADA VACUNO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>10.73</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CEBOLLA BLANCA</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CEBOLLETA </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>manojo</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CEREZAS</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CERVEZA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CERVEZA 0</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CHAMPIÑON ENTERO CONSERVA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>6.11</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CHAMPIÑONES</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CIRUELAS </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>COGOLLOS CORAZONES</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>COLIFROR</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CORVINA FRESCA ENTERA</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>DENTRIFICO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>DESENGRASANTE  KH-7</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>DETERGENTE LIQUIDO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>dosis</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>DORADA FRESCA ENTERA</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="E43" t="n">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ENTRECOT</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>26.45</v>
+      </c>
+      <c r="E44" t="n">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ESPAGUETI PASTA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESPARRAGO BLANCO MUY GRUESO 6/12 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>23.92</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ESPINACAS</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ESPUMA AFEITAR</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>FAIRY</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>GARBANZO COCIDO</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GEL BAÑO </t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>GUINDILLAS</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>11.08</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>GUISANTE CONSERVA</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GULAS </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>23.79</v>
+      </c>
+      <c r="E54" t="n">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HAMBURGUESA VACUNO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="E55" t="n">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>HAMBURGUESA VACUNO/CERDO</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>HARINA TRIGO</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HUEVOS CAMPEROS </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HUEVOS CODORNIZ</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HUEVOS XL</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>JAMON COCIDO EXTRA LONCHAS</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JUDIA VERDE PLANA </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>KETCHUP</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>KIWI VERDE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LANGOSTINO </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="E65" t="n">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LANGOSTINO COCIDO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="E66" t="n">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LAVAVAJILLAS MAQUINA GEL </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="E67" t="n">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>LECHE DESNATADA</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>LECHE SEMIDESNATADA</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LECHUGA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LEGIA </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="E71" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>LENTEJA PARDINA</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="E72" t="n">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>LIMON</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LIMPIACRISTALES</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LIMPIADOR SUELO</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LIMPIADOR VITROCERAMICA </t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>LONGANIZA FRESCO</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>5.32</v>
+      </c>
+      <c r="E77" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LUBINA FRESCA ENTERA </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="E78" t="n">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MACARRON PASTA DE TRIGO</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MANDARINA</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MANTEQUILLA </t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="E81" t="n">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MANZANA FUYI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>MANZANA GOLDEN</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>MAYONESA</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>5.23</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEJILLON ESCABECHE 8/12 PIEZAS EN ACEITE OLIVA </t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E85" t="n">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MEJILLON FRESCO</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MELOCOTON </t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MELON</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MENESTRA VERDURA CONSERVA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MERLUZA FRESCA ENTERA </t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>9.949999999999999</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MOSTAZA</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>NARANJA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NATA COCINA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NUEZ </t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>21.94</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>PANCETA LONCHAS</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>16.33</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PAÑUELOS PAPEL BOLSILLO</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PAPEL ALUMINIO </t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>metro</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>PAPEL COCINA BLANCO DOBLE</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>rollo</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>PAPEL HIGIENICO DOBLE ROLLO 2 CAPAS</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>rollo</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.37</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fixed error with paths
</commit_message>
<xml_diff>
--- a/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
+++ b/src/price_tracker/outputs/01_listado_precios_Enero.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_02" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_03" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_10" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_01_15" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2023_01_02" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2023_01_03" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2023_01_10" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2023_01_15" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2023_01_21" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -9271,7 +9272,6 @@
           <t>BONITO CONSERVA</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
         <v>0</v>
       </c>
@@ -9477,7 +9477,6 @@
           <t>CEREZAS</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr"/>
       <c r="D31" t="n">
         <v>0</v>
       </c>
@@ -9578,7 +9577,6 @@
           <t xml:space="preserve">CIRUELAS </t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
       <c r="D36" t="n">
         <v>0</v>
       </c>
@@ -9637,7 +9635,6 @@
           <t>CORVINA FRESCA ENTERA</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
         <v>0</v>
       </c>
@@ -9801,7 +9798,6 @@
           <t>ESPINACAS</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr"/>
       <c r="D47" t="n">
         <v>0</v>
       </c>
@@ -9881,7 +9877,6 @@
           <t xml:space="preserve">GEL BAÑO </t>
         </is>
       </c>
-      <c r="C51" t="inlineStr"/>
       <c r="D51" t="n">
         <v>0</v>
       </c>
@@ -10402,7 +10397,6 @@
           <t xml:space="preserve">LIMPIADOR VITROCERAMICA </t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
       <c r="D76" t="n">
         <v>0</v>
       </c>
@@ -10608,7 +10602,6 @@
           <t>MEJILLON FRESCO</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr"/>
       <c r="D86" t="n">
         <v>0</v>
       </c>
@@ -11234,7 +11227,6 @@
           <t xml:space="preserve">QUESO EMMENTAL </t>
         </is>
       </c>
-      <c r="C116" t="inlineStr"/>
       <c r="D116" t="n">
         <v>0</v>
       </c>
@@ -11272,7 +11264,6 @@
           <t>QUESO GOUDA TIERNO,</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr"/>
       <c r="D118" t="n">
         <v>0</v>
       </c>
@@ -11331,7 +11322,6 @@
           <t xml:space="preserve">SALMON FRESCO </t>
         </is>
       </c>
-      <c r="C121" t="inlineStr"/>
       <c r="D121" t="n">
         <v>0</v>
       </c>
@@ -11600,7 +11590,6 @@
           <t>ZUMO NARANJA</t>
         </is>
       </c>
-      <c r="C134" t="inlineStr"/>
       <c r="D134" t="n">
         <v>0</v>
       </c>
@@ -11624,6 +11613,2806 @@
       </c>
       <c r="D135" t="n">
         <v>0.8</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E135"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PRODUCTOS</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>UNIDADES</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Eroski</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>BM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ABRILLANTADOR LAVAVAJILLAS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ACEITE GIRASOL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7.97</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ACEITUNA NEGRA SIN HUESO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>13</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.07</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ACEITUNA RELLENA ANCHOA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AGUACATE </t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AJO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALCACHOFA CORAZONES GRANDES </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>15.48</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALMENDRA CRUDA </t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>15.03</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ALUBIA COCIDA BLANCA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ANCHOA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>18</v>
+      </c>
+      <c r="E12" t="n">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ANCHOA FILETE ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ARANDANOS </t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ARROZ BOMBA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>5.63</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ATUN CLARO EN ACEITE OLIVA </t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AVELLANA TOSTADA PELADA SIN SA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>20.33</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.49</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AZUCAR BLANQUILLA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BOLSA BASURA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BONITO </t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BONITO CONSERVA</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BORRAJA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5.78</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BROCOLI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CACAHUETE TOSTADO </t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CALABACIN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CALABAZA</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CALABAZA CACAHUETE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CARNE PICADA VACUNO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CEBOLLA BLANCA</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CEBOLLETA </t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>manojo</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CEREZAS</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CERVEZA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CERVEZA 0</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CHAMPIÑON ENTERO CONSERVA</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>6.11</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CHAMPIÑONES</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CIRUELAS </t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>COGOLLOS CORAZONES</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>COLIFROR</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CORVINA FRESCA ENTERA</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>DENTRIFICO</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>DESENGRASANTE  KH-7</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>DETERGENTE LIQUIDO</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>dosis</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>DORADA FRESCA ENTERA</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="E43" t="n">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ENTRECOT</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>26.45</v>
+      </c>
+      <c r="E44" t="n">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ESPAGUETI PASTA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ESPARRAGO BLANCO MUY GRUESO 6/12 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>23.92</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ESPINACAS</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ESPUMA AFEITAR</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>FAIRY</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>GARBANZO COCIDO</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GEL BAÑO </t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>GUINDILLAS</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>11.08</v>
+      </c>
+      <c r="E52" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>GUISANTE CONSERVA</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GULAS </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>23.79</v>
+      </c>
+      <c r="E54" t="n">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>HAMBURGUESA VACUNO</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="E55" t="n">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>HAMBURGUESA VACUNO/CERDO</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>HARINA TRIGO</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HUEVOS CAMPEROS </t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>HUEVOS CODORNIZ</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>HUEVOS XL</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>docena</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>JAMON COCIDO EXTRA LONCHAS</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JUDIA VERDE PLANA </t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>KETCHUP</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>KIWI VERDE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="E64" t="n">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LANGOSTINO </t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="E65" t="n">
+        <v>13.99</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>LANGOSTINO COCIDO</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="E66" t="n">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LAVAVAJILLAS MAQUINA GEL </t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="E67" t="n">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>LECHE DESNATADA</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>LECHE SEMIDESNATADA</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LECHUGA</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LEGIA </t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E71" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>LENTEJA PARDINA</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="E72" t="n">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>LIMON</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LIMPIACRISTALES</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LIMPIADOR SUELO</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LIMPIADOR VITROCERAMICA </t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>LONGANIZA FRESCO</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>5.32</v>
+      </c>
+      <c r="E77" t="n">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LUBINA FRESCA ENTERA </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="E78" t="n">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>MACARRON PASTA DE TRIGO</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>MANDARINA</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MANTEQUILLA </t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="E81" t="n">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MANZANA FUYI</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>MANZANA GOLDEN</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>MAYONESA</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEJILLON ESCABECHE 8/12 PIEZAS EN ACEITE OLIVA </t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="E85" t="n">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>MEJILLON FRESCO</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MELOCOTON </t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>MELON</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>MENESTRA VERDURA CONSERVA</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>10.24</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MERLUZA FRESCA ENTERA </t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>9.949999999999999</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>MOSTAZA</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>8.75</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>NARANJA</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NATA COCINA</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NUEZ </t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>21.94</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>PANCETA LONCHAS</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>16.33</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PAÑUELOS PAPEL BOLSILLO</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>unidad</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PAPEL ALUMINIO </t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>metro</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>PAPEL COCINA BLANCO DOBLE</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>rollo</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>PAPEL HIGIENICO DOBLE ROLLO 2 CAPAS</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>rollo</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>PATATA ENTERA CONSERVA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>PATATA NUEVA</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PAVO </t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>19.13</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PECHUGA PAVO </t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>14.95</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>PEPINILLOS</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>14.54</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>PIMIENTO ASADO TIRAS</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PIMIENTO ITALIANO </t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>PIMIENTO PIQUILLO ASADO ENTERO</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>PIMIENTO ROJO</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>PIÑA</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>PIPAS GIRASOL GIGANTES TOSTADAS CON SAL</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>15.64</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>PLATANO CANARIO</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>POCHA  COCIDA</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>7.78</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>POLLO ENTERO LIMPIO FRESCO</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>POLLO PECHUGA FILETES FRESCO</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>12.34</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PUERRO </t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QUESO EMMENTAL </t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">QUESO FRESCO </t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>13.17</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>QUESO GOUDA TIERNO,</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">REPOLLO </t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>SALMON AHUMADO LONCHAS</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SALMON FRESCO </t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SALSA BECHAMEL </t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>SARDINA ACEITE OLIVA</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>13.83</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUAVIZANTE ROPA CONCENTRADO </t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>dosis</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>TALLARINES</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>TOMATE  CHERRY</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>TOMATE ENSALADA</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>TOMATE FRITO ACEITE OLIVA RECETA ARTESANA</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>TOMATE PERA</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>VINAGRE BALSAMICO MODENA</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>VINAGRE JEREZ</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>7.96</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>YOGUR GRIEGO NATURAL</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>6.09</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>ZANAHORIA</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>kilo</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>ZUMO NARANJA</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JABON MANOS LIQUIDO </t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>mililitro</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>0.9</v>
       </c>
       <c r="E135" t="n">
         <v>0</v>

</xml_diff>